<commit_message>
Updates to html to correct $(initfn) syntax. Add new adbpush-tables-tablesdemo grunt command. Add app.properties.tablesdemo to auto-set tables home screen and demo server.
</commit_message>
<xml_diff>
--- a/app/config/tables/femaleClients/forms/addClient/addClient.xlsx
+++ b/app/config/tables/femaleClients/forms/addClient/addClient.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\toolsuite\app-designer\app\config\tables\femaleClients\forms\addClient\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="0" windowWidth="25600" windowHeight="16080" tabRatio="500"/>
+    <workbookView xWindow="1126" yWindow="0" windowWidth="25606" windowHeight="16076" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="107">
   <si>
     <t>type</t>
   </si>
@@ -43,9 +48,6 @@
   </si>
   <si>
     <t>default</t>
-  </si>
-  <si>
-    <t>relevant</t>
   </si>
   <si>
     <t>read_only</t>
@@ -352,7 +354,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1733,6 +1735,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -2059,46 +2064,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.1640625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="39.1640625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="39.109375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="39.109375" style="8" customWidth="1"/>
     <col min="3" max="3" width="23" style="12" customWidth="1"/>
     <col min="4" max="4" width="63" style="3" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" style="3" customWidth="1"/>
-    <col min="6" max="7" width="10.83203125" style="3"/>
-    <col min="8" max="8" width="10.83203125" style="14"/>
-    <col min="9" max="9" width="10.83203125" style="3"/>
+    <col min="5" max="5" width="22.77734375" style="3" customWidth="1"/>
+    <col min="6" max="7" width="10.77734375" style="3"/>
+    <col min="8" max="8" width="10.77734375" style="14"/>
+    <col min="9" max="9" width="10.77734375" style="3"/>
     <col min="10" max="10" width="15" style="3" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" style="3"/>
-    <col min="12" max="12" width="28" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="3"/>
+    <col min="11" max="16384" width="10.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="30">
+    <row r="1" spans="1:15" ht="31.45" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>2</v>
@@ -2113,7 +2116,7 @@
         <v>5</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>6</v>
@@ -2122,61 +2125,58 @@
         <v>7</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="47.15" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="C2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="45">
-      <c r="A2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H2" s="21" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3" s="22" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H4" s="22" t="b">
         <v>1</v>
@@ -2201,53 +2201,53 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="21.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="21.5" style="2"/>
+    <col min="1" max="1" width="23.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="21.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
     </row>
-    <row r="76" spans="3:3">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C76" s="5"/>
     </row>
   </sheetData>
@@ -2269,55 +2269,55 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="2"/>
+    <col min="4" max="16384" width="10.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="B3" s="2">
         <v>20140512</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -2339,14 +2339,14 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.83203125" customWidth="1"/>
+    <col min="1" max="1" width="30.77734375" customWidth="1"/>
     <col min="2" max="2" width="25.33203125" customWidth="1"/>
     <col min="3" max="3" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -2354,516 +2354,516 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="16" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="18" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="18" t="s">
+      <c r="B7" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="18" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="18" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="18" t="s">
+      <c r="B10" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="18" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="18" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="18" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="18" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="18" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="18" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="18" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="18" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="18" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="18" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="18" t="s">
+      <c r="B18" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="18" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="18" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="18" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="18" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="18" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="18" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="18" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="18" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="18" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="18" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="18" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="18" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="18" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="18" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="18" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="18" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="18" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="18" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28" s="18" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="18" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" s="18" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="18" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" s="18" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="18" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31" s="18" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="18" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B32" s="18" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="18" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="18" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="18" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="18" t="s">
+      <c r="B34" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="18" t="s">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="B35" s="18" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="18" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B36" s="18" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="18" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B37" s="18" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B38" s="18" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B39" s="18" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B40" s="18" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="18" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B41" s="18" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" s="18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B42" s="18" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="18" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B43" s="18" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="18" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B44" s="18" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" s="18" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B45" s="18" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="19" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B46" s="19" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="19" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B47" s="19" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" s="20" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B48" s="20" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49" s="20" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B49" s="20" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" s="20" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B50" s="20" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" s="20" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B51" s="20" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52" s="20" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B52" s="20" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B53" s="20" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="B53" s="20" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" s="20" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B54" s="20" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B55" s="20" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B55" s="20" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" s="20" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="B56" s="20" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B57" s="20" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B57" s="20" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58" s="20" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B58" s="20" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B59" s="20" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B59" s="20" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B60" s="20" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B60" s="20" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B61" s="20" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B61" s="20" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B62" s="20" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B62" s="20" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B63" s="20" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B63" s="20" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="20" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="20" t="s">
+      <c r="B64" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="B64" s="20" t="s">
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B65" s="20" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B65" s="20" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Name change hope study form
</commit_message>
<xml_diff>
--- a/app/config/tables/femaleClients/forms/addClient/addClient.xlsx
+++ b/app/config/tables/femaleClients/forms/addClient/addClient.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\toolsuite\app-designer\app\config\tables\femaleClients\forms\addClient\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1126" yWindow="0" windowWidth="25606" windowHeight="16076" tabRatio="500"/>
+    <workbookView xWindow="1120" yWindow="0" windowWidth="25600" windowHeight="16080" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -102,9 +97,6 @@
     <t>Control</t>
   </si>
   <si>
-    <t>Add Client Form</t>
-  </si>
-  <si>
     <t>values_list</t>
   </si>
   <si>
@@ -349,12 +341,15 @@
   </si>
   <si>
     <t>interviewer_init</t>
+  </si>
+  <si>
+    <t>Add Client Brief</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2066,42 +2061,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="39.109375" style="10" customWidth="1"/>
-    <col min="2" max="2" width="39.109375" style="8" customWidth="1"/>
+    <col min="1" max="1" width="39.1640625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="39.1640625" style="8" customWidth="1"/>
     <col min="3" max="3" width="23" style="12" customWidth="1"/>
     <col min="4" max="4" width="63" style="3" customWidth="1"/>
-    <col min="5" max="5" width="22.77734375" style="3" customWidth="1"/>
-    <col min="6" max="7" width="10.77734375" style="3"/>
-    <col min="8" max="8" width="10.77734375" style="14"/>
-    <col min="9" max="9" width="10.77734375" style="3"/>
+    <col min="5" max="5" width="22.83203125" style="3" customWidth="1"/>
+    <col min="6" max="7" width="10.83203125" style="3"/>
+    <col min="8" max="8" width="10.83203125" style="14"/>
+    <col min="9" max="9" width="10.83203125" style="3"/>
     <col min="10" max="10" width="15" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="10.77734375" style="3"/>
+    <col min="11" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="30">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>2</v>
@@ -2134,12 +2129,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="47.15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="45">
       <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>13</v>
@@ -2151,12 +2146,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15">
       <c r="A3" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>14</v>
@@ -2165,15 +2160,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15">
       <c r="A4" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>15</v>
@@ -2201,25 +2196,25 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="21.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="21.44140625" style="2"/>
+    <col min="1" max="1" width="23.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="21.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -2230,7 +2225,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -2241,13 +2236,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="B15" s="4"/>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:3">
       <c r="C76" s="5"/>
     </row>
   </sheetData>
@@ -2265,30 +2260,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="10.77734375" style="2"/>
+    <col min="4" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -2296,28 +2291,28 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2">
         <v>20140512</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2339,14 +2334,14 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="30.77734375" customWidth="1"/>
+    <col min="1" max="1" width="30.83203125" customWidth="1"/>
     <col min="2" max="2" width="25.33203125" customWidth="1"/>
     <col min="3" max="3" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -2354,516 +2349,516 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="16" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="16" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="18" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="B7" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="18" t="s">
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="18" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" s="18" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
+      <c r="B10" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="18" t="s">
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="18" t="s">
+    <row r="12" spans="1:2">
+      <c r="A12" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="18" t="s">
+    <row r="13" spans="1:2">
+      <c r="A13" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="18" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="18" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="18" t="s">
+    <row r="15" spans="1:2">
+      <c r="A15" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="18" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="18" t="s">
+    <row r="16" spans="1:2">
+      <c r="A16" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="18" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="18" t="s">
+    <row r="18" spans="1:2">
+      <c r="A18" s="18" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="18" t="s">
+      <c r="B18" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="18" t="s">
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="18" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="18" t="s">
+    <row r="21" spans="1:2">
+      <c r="A21" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="18" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2">
       <c r="A22" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="18" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="18" t="s">
+    <row r="24" spans="1:2">
+      <c r="A24" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="18" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="18" t="s">
+    <row r="25" spans="1:2">
+      <c r="A25" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="18" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="18" t="s">
+    <row r="26" spans="1:2">
+      <c r="A26" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="18" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="18" t="s">
+    <row r="27" spans="1:2">
+      <c r="A27" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="18" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="18" t="s">
+    <row r="28" spans="1:2">
+      <c r="A28" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="18" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2">
       <c r="A29" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B29" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="18" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B30" s="18" t="s">
+    <row r="31" spans="1:2">
+      <c r="A31" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="18" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="18" t="s">
+    <row r="32" spans="1:2">
+      <c r="A32" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="18" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="18" t="s">
+    <row r="33" spans="1:2">
+      <c r="A33" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="18" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="18" t="s">
+    <row r="34" spans="1:2">
+      <c r="A34" s="18" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="18" t="s">
+      <c r="B34" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="18" t="s">
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="18" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" s="18" t="s">
+    <row r="36" spans="1:2">
+      <c r="A36" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B36" s="18" t="s">
+    <row r="37" spans="1:2">
+      <c r="A37" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" s="18" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="18" t="s">
+    <row r="38" spans="1:2">
+      <c r="A38" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="18" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38" s="18" t="s">
+    <row r="39" spans="1:2">
+      <c r="A39" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B39" s="18" t="s">
+    <row r="40" spans="1:2">
+      <c r="A40" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B40" s="18" t="s">
+    <row r="41" spans="1:2">
+      <c r="A41" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B41" s="18" t="s">
+    <row r="42" spans="1:2">
+      <c r="A42" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B42" s="18" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B42" s="18" t="s">
+    <row r="43" spans="1:2">
+      <c r="A43" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B43" s="18" t="s">
+    <row r="44" spans="1:2">
+      <c r="A44" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="18" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B44" s="18" t="s">
+    <row r="45" spans="1:2">
+      <c r="A45" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" s="18" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B45" s="18" t="s">
+    <row r="46" spans="1:2">
+      <c r="A46" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" s="19" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B46" s="19" t="s">
+    <row r="47" spans="1:2">
+      <c r="A47" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47" s="19" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B47" s="19" t="s">
+    <row r="48" spans="1:2">
+      <c r="A48" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48" s="20" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B48" s="20" t="s">
+    <row r="49" spans="1:2">
+      <c r="A49" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" s="20" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B49" s="20" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2">
       <c r="A50" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B50" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" s="20" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B51" s="20" t="s">
+    <row r="52" spans="1:2">
+      <c r="A52" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B52" s="20" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B52" s="20" t="s">
+    <row r="53" spans="1:2">
+      <c r="A53" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53" s="20" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B53" s="20" t="s">
+    <row r="54" spans="1:2">
+      <c r="A54" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54" s="20" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B54" s="20" t="s">
+    <row r="55" spans="1:2">
+      <c r="A55" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B55" s="20" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B55" s="20" t="s">
+    <row r="56" spans="1:2">
+      <c r="A56" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B56" s="20" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B56" s="20" t="s">
+    <row r="57" spans="1:2">
+      <c r="A57" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B57" s="20" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B57" s="20" t="s">
+    <row r="58" spans="1:2">
+      <c r="A58" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B58" s="20" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B58" s="20" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2">
       <c r="A59" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B59" s="20" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
       <c r="A60" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B60" s="20" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
       <c r="A61" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B61" s="20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B62" s="20" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B62" s="20" t="s">
+    <row r="63" spans="1:2">
+      <c r="A63" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B63" s="20" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B63" s="20" t="s">
+    <row r="64" spans="1:2">
+      <c r="A64" s="20" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="20" t="s">
+      <c r="B64" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="B64" s="20" t="s">
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B65" s="20" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B65" s="20" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>